<commit_message>
add re-run results of x264_s to the table
</commit_message>
<xml_diff>
--- a/documentation/spec/logs/results.xlsx
+++ b/documentation/spec/logs/results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E2C709-A963-0E4D-A0EF-9A32108979E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9665F19C-C274-F14C-8FFA-0726051247EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19760" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19760" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
   <sheets>
     <sheet name="127, 128" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>SPEC CPU 2017</t>
   </si>
@@ -145,14 +145,20 @@
     <t>--size=ref --noreportable as 600.perlbench_s crashes for test.</t>
   </si>
   <si>
-    <t>Run crashed</t>
+    <t>Base Score**</t>
+  </si>
+  <si>
+    <t>**:</t>
+  </si>
+  <si>
+    <t>Not accurate, as the 625.x264_s data is from a separate run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,14 +198,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -390,16 +388,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,12 +402,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -452,13 +438,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -777,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2E7EA3-8BF5-F743-9E89-1A0A4F76CDF3}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,282 +784,285 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="27" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="9">
         <v>3061</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="16">
         <v>10930</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="17">
         <v>0.16200000000000001</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="28">
         <f>D5/B5</f>
         <v>3.5707285200914733</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>3390</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>1.17</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="18">
         <v>9301</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="19">
         <v>0.42799999999999999</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="29">
         <f>D6/B6</f>
         <v>2.7436578171091446</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>3182</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>1.48</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="18">
         <v>3654</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="19">
         <v>1.29</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="29">
         <f t="shared" ref="F7:F14" si="0">D7/B7</f>
         <v>1.1483343808925204</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>2576</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>0.63300000000000001</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="18">
         <v>8210</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="19">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>3.1871118012422359</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>1711</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>0.82799999999999996</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="18">
         <v>4563</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="19">
         <v>0.311</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="29">
         <f t="shared" si="0"/>
         <v>2.6668614845119811</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>2921</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>0.60399999999999998</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37" t="s">
-        <v>29</v>
+      <c r="D10" s="18">
+        <v>4333</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="F10" s="29">
+        <f t="shared" si="0"/>
+        <v>1.4833960972269771</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>2459</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>0.58299999999999996</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="18">
         <v>10330</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="19">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="29">
         <f t="shared" si="0"/>
         <v>4.2008946726311507</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>3171</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>0.53800000000000003</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="18">
         <v>7517</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="19">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="29">
         <f t="shared" si="0"/>
         <v>2.3705455692210657</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>2213</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <v>1.33</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="18">
         <v>4891</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="19">
         <v>0.60099999999999998</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="29">
         <f t="shared" si="0"/>
         <v>2.2101220063262539</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="13">
         <v>8915</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="14">
         <v>0.69299999999999995</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="20">
         <v>12625</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="21">
         <v>0.49</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="0"/>
         <v>1.4161525518788558</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="28" t="s">
+      <c r="C15" s="33"/>
+      <c r="D15" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="4">
+      <c r="B16" s="34">
         <v>0.78810000000000002</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34">
         <v>0.3337</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="29">
+      <c r="E16" s="34"/>
+      <c r="F16" s="25">
         <f>B16/D16</f>
         <v>2.3617021276595747</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
@@ -1079,7 +1071,7 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
@@ -1088,7 +1080,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
@@ -1097,7 +1089,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
@@ -1118,6 +1110,12 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1127,14 +1125,13 @@
       <c r="G27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>